<commit_message>
added final GSA results and final plots, including the ones for robust case with lifetime normal and uniform
</commit_message>
<xml_diff>
--- a/generated_files/gsa_results/cge_N500/sobol_first.xlsx
+++ b/generated_files/gsa_results/cge_N500/sobol_first.xlsx
@@ -1,29 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andpa\OneDrive - University College London\S4CE\GSA\Geothermal\generated_files\gsa_results\cge_N500\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_FFC65FC05D092EECB0170B230309495B68C4DDC5" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{8D690604-B79D-44B3-A696-196C43E4C8B7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -135,8 +121,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,14 +185,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -253,7 +231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,27 +263,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -337,24 +297,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -530,16 +472,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:R18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -600,55 +540,55 @@
         <v>17</v>
       </c>
       <c r="C2">
-        <v>2.2418850428119648E-3</v>
+        <v>0.002241525188300966</v>
       </c>
       <c r="D2">
-        <v>0.60236359572503684</v>
+        <v>0.6023872789225153</v>
       </c>
       <c r="E2">
-        <v>0.57821463335067236</v>
+        <v>0.5782372294856711</v>
       </c>
       <c r="F2">
-        <v>0.59689541373829758</v>
+        <v>0.5969191903245424</v>
       </c>
       <c r="G2">
-        <v>0.56536320813902552</v>
+        <v>0.5653853608835668</v>
       </c>
       <c r="H2">
-        <v>0.56125722820631752</v>
+        <v>0.5612790061240372</v>
       </c>
       <c r="I2">
-        <v>0.63329772479909419</v>
+        <v>0.6333219318506984</v>
       </c>
       <c r="J2">
-        <v>0.57557774046288124</v>
+        <v>0.5756001595903323</v>
       </c>
       <c r="K2">
-        <v>0.56927899873982246</v>
+        <v>0.5693018565930538</v>
       </c>
       <c r="L2">
-        <v>0.60982081482343298</v>
+        <v>0.6098451175380967</v>
       </c>
       <c r="M2">
-        <v>0.55137083234824347</v>
+        <v>0.5513922316510679</v>
       </c>
       <c r="N2">
-        <v>0.55184357119240757</v>
+        <v>0.5518649080224552</v>
       </c>
       <c r="O2">
-        <v>0.65859783917646175</v>
+        <v>0.6586234369390446</v>
       </c>
       <c r="P2">
-        <v>0.6269393549088067</v>
+        <v>0.6269641386976519</v>
       </c>
       <c r="Q2">
-        <v>0.60045489330251434</v>
+        <v>0.6004783478921585</v>
       </c>
       <c r="R2">
-        <v>0.63953672682492613</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.6395612591289889</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -656,55 +596,55 @@
         <v>18</v>
       </c>
       <c r="C3">
-        <v>2.6095705592476962E-3</v>
+        <v>0.002609389096876603</v>
       </c>
       <c r="D3">
-        <v>0.20349389661528461</v>
+        <v>0.2034944059642876</v>
       </c>
       <c r="E3">
-        <v>0.2148615601713757</v>
+        <v>0.2148628105378421</v>
       </c>
       <c r="F3">
-        <v>0.210453826630466</v>
+        <v>0.2104544075071044</v>
       </c>
       <c r="G3">
-        <v>0.223549785208777</v>
+        <v>0.2235511428259462</v>
       </c>
       <c r="H3">
-        <v>0.22567421916722549</v>
+        <v>0.2256755705468588</v>
       </c>
       <c r="I3">
-        <v>0.1660924663107442</v>
+        <v>0.1660930026428964</v>
       </c>
       <c r="J3">
-        <v>0.21490992365994771</v>
+        <v>0.2149112221367634</v>
       </c>
       <c r="K3">
-        <v>0.23938616061440571</v>
+        <v>0.2393866689605409</v>
       </c>
       <c r="L3">
-        <v>0.19615670648917019</v>
+        <v>0.1961572523465677</v>
       </c>
       <c r="M3">
-        <v>0.23157349258663609</v>
+        <v>0.2315749402354579</v>
       </c>
       <c r="N3">
-        <v>0.2306037938649439</v>
+        <v>0.2306052318165816</v>
       </c>
       <c r="O3">
-        <v>0.1554847919485299</v>
+        <v>0.1554851683628184</v>
       </c>
       <c r="P3">
-        <v>0.17345566148577621</v>
+        <v>0.173456102395718</v>
       </c>
       <c r="Q3">
-        <v>0.19946078179103879</v>
+        <v>0.1994615707716725</v>
       </c>
       <c r="R3">
-        <v>0.1608609232337492</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.1608613607950664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -712,55 +652,55 @@
         <v>19</v>
       </c>
       <c r="C4">
-        <v>1.8275938917868171E-5</v>
+        <v>1.827291917466211E-05</v>
       </c>
       <c r="D4">
-        <v>3.7838726867427449E-3</v>
+        <v>0.003783836995179485</v>
       </c>
       <c r="E4">
-        <v>2.3302190319571211E-3</v>
+        <v>0.002330147909654209</v>
       </c>
       <c r="F4">
-        <v>3.1483377629438979E-3</v>
+        <v>0.003148297859696607</v>
       </c>
       <c r="G4">
-        <v>1.5867048083888021E-3</v>
+        <v>0.001586643664938069</v>
       </c>
       <c r="H4">
-        <v>1.437092622703078E-3</v>
+        <v>0.001437037941948919</v>
       </c>
       <c r="I4">
-        <v>7.9824671611154596E-3</v>
+        <v>0.007982390895899444</v>
       </c>
       <c r="J4">
-        <v>2.299731263832332E-3</v>
+        <v>0.002299656063199037</v>
       </c>
       <c r="K4">
-        <v>1.0945458390307289E-3</v>
+        <v>0.001094521085065529</v>
       </c>
       <c r="L4">
-        <v>4.5021002164615468E-3</v>
+        <v>0.004502046633580938</v>
       </c>
       <c r="M4">
-        <v>9.9883148667533257E-4</v>
+        <v>0.0009987862843260746</v>
       </c>
       <c r="N4">
-        <v>1.057690557770027E-3</v>
+        <v>0.001057643374525995</v>
       </c>
       <c r="O4">
-        <v>4.368309320199785E-3</v>
+        <v>0.004368149760455262</v>
       </c>
       <c r="P4">
-        <v>6.9565890589845464E-3</v>
+        <v>0.006956529036764805</v>
       </c>
       <c r="Q4">
-        <v>3.87159680610215E-3</v>
+        <v>0.003871518769012676</v>
       </c>
       <c r="R4">
-        <v>8.9899996714686691E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.008989902255070579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -768,55 +708,55 @@
         <v>20</v>
       </c>
       <c r="C5">
-        <v>2.2458179549834299E-4</v>
+        <v>0.0002246018517667613</v>
       </c>
       <c r="D5">
-        <v>4.9200361929132566E-3</v>
+        <v>0.004903577015905084</v>
       </c>
       <c r="E5">
-        <v>4.5723971939179578E-3</v>
+        <v>0.004556830912441726</v>
       </c>
       <c r="F5">
-        <v>4.8064834994411137E-3</v>
+        <v>0.004789878487614359</v>
       </c>
       <c r="G5">
-        <v>4.4510561061064709E-3</v>
+        <v>0.00443591325262542</v>
       </c>
       <c r="H5">
-        <v>4.5986756384125893E-3</v>
+        <v>0.004583960336442401</v>
       </c>
       <c r="I5">
-        <v>4.3757289709640797E-3</v>
+        <v>0.004358450474797501</v>
       </c>
       <c r="J5">
-        <v>4.4948635471319187E-3</v>
+        <v>0.004479381130663515</v>
       </c>
       <c r="K5">
-        <v>4.7877012977502152E-3</v>
+        <v>0.004771978546679033</v>
       </c>
       <c r="L5">
-        <v>4.4857751405532921E-3</v>
+        <v>0.004468607657983305</v>
       </c>
       <c r="M5">
-        <v>4.5289880955872251E-3</v>
+        <v>0.004514598717481447</v>
       </c>
       <c r="N5">
-        <v>4.5411215928707069E-3</v>
+        <v>0.004526760118896634</v>
       </c>
       <c r="O5">
-        <v>3.253263381842484E-3</v>
+        <v>0.003233696604310065</v>
       </c>
       <c r="P5">
-        <v>4.1389525036875808E-3</v>
+        <v>0.004121554897500613</v>
       </c>
       <c r="Q5">
-        <v>4.3858297719538896E-3</v>
+        <v>0.004369633605941657</v>
       </c>
       <c r="R5">
-        <v>4.0018249049537259E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.003983821798928894</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -824,7 +764,7 @@
         <v>21</v>
       </c>
       <c r="C6">
-        <v>0.94887670087112375</v>
+        <v>0.9488769725732813</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -872,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -880,55 +820,55 @@
         <v>22</v>
       </c>
       <c r="C7">
-        <v>1.135176936145739E-4</v>
+        <v>0.0001134978219381413</v>
       </c>
       <c r="D7">
-        <v>4.1178653273037814E-3</v>
+        <v>0.004114754517157503</v>
       </c>
       <c r="E7">
-        <v>4.1293489391450167E-3</v>
+        <v>0.004126410679297526</v>
       </c>
       <c r="F7">
-        <v>4.633933953223892E-3</v>
+        <v>0.004630718262849533</v>
       </c>
       <c r="G7">
-        <v>4.1738148192634076E-3</v>
+        <v>0.004170972531386218</v>
       </c>
       <c r="H7">
-        <v>3.661687513869959E-3</v>
+        <v>0.003659040270726393</v>
       </c>
       <c r="I7">
-        <v>4.5951859935523922E-3</v>
+        <v>0.004591708633793756</v>
       </c>
       <c r="J7">
-        <v>4.1432181155316907E-3</v>
+        <v>0.004140288257948376</v>
       </c>
       <c r="K7">
-        <v>4.54765420103971E-3</v>
+        <v>0.004544726594529571</v>
       </c>
       <c r="L7">
-        <v>5.248611629061658E-3</v>
+        <v>0.005245122188450216</v>
       </c>
       <c r="M7">
-        <v>3.70244275402664E-3</v>
+        <v>0.003699870485485699</v>
       </c>
       <c r="N7">
-        <v>3.6161598623562739E-3</v>
+        <v>0.003613606972182979</v>
       </c>
       <c r="O7">
-        <v>9.1832302913030274E-3</v>
+        <v>0.009178623935878</v>
       </c>
       <c r="P7">
-        <v>5.4491581790849447E-3</v>
+        <v>0.005445503886342891</v>
       </c>
       <c r="Q7">
-        <v>4.2042887477512338E-3</v>
+        <v>0.004201159795657701</v>
       </c>
       <c r="R7">
-        <v>5.8668408010842362E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.005862988596105665</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -936,55 +876,55 @@
         <v>23</v>
       </c>
       <c r="C8">
-        <v>8.2059573034460427E-5</v>
+        <v>8.204745374811053E-05</v>
       </c>
       <c r="D8">
-        <v>2.0483070063980662E-3</v>
+        <v>0.002048238172798282</v>
       </c>
       <c r="E8">
-        <v>1.871157130141314E-3</v>
+        <v>0.00187109990510739</v>
       </c>
       <c r="F8">
-        <v>2.0258073536576051E-3</v>
+        <v>0.002025751871825456</v>
       </c>
       <c r="G8">
-        <v>1.764231931222048E-3</v>
+        <v>0.001764173263960969</v>
       </c>
       <c r="H8">
-        <v>1.697808199911541E-3</v>
+        <v>0.001697736112932474</v>
       </c>
       <c r="I8">
-        <v>2.2889988508282859E-3</v>
+        <v>0.002288956068968809</v>
       </c>
       <c r="J8">
-        <v>1.8475954119592469E-3</v>
+        <v>0.001847542170097934</v>
       </c>
       <c r="K8">
-        <v>1.755285927337041E-3</v>
+        <v>0.001755229358986496</v>
       </c>
       <c r="L8">
-        <v>2.1663294412419499E-3</v>
+        <v>0.002166292243978485</v>
       </c>
       <c r="M8">
-        <v>1.606686750056825E-3</v>
+        <v>0.00160661372423862</v>
       </c>
       <c r="N8">
-        <v>1.6033905882876179E-3</v>
+        <v>0.001603317644580435</v>
       </c>
       <c r="O8">
-        <v>2.3227683716825539E-3</v>
+        <v>0.002322861720208964</v>
       </c>
       <c r="P8">
-        <v>2.368588656778864E-3</v>
+        <v>0.002368544496389399</v>
       </c>
       <c r="Q8">
-        <v>2.086099867353032E-3</v>
+        <v>0.002086046324721072</v>
       </c>
       <c r="R8">
-        <v>2.3007469143390869E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.002300755851295236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -992,55 +932,55 @@
         <v>24</v>
       </c>
       <c r="C9">
-        <v>5.2338916083310087E-6</v>
+        <v>5.235293234865941E-06</v>
       </c>
       <c r="D9">
-        <v>2.6990040777613258E-4</v>
+        <v>0.0002699466308320415</v>
       </c>
       <c r="E9">
-        <v>2.5839784037221518E-4</v>
+        <v>0.0002584342203071563</v>
       </c>
       <c r="F9">
-        <v>2.593382871186004E-4</v>
+        <v>0.0002593838213818261</v>
       </c>
       <c r="G9">
-        <v>2.3855992948508621E-4</v>
+        <v>0.0002385917748235055</v>
       </c>
       <c r="H9">
-        <v>2.289373700799484E-4</v>
+        <v>0.0002289660279254155</v>
       </c>
       <c r="I9">
-        <v>3.6841835783520089E-4</v>
+        <v>0.0003684808201916695</v>
       </c>
       <c r="J9">
-        <v>2.5790146807527748E-4</v>
+        <v>0.0002579371303632944</v>
       </c>
       <c r="K9">
-        <v>1.8847257874710771E-4</v>
+        <v>0.0001885067931063198</v>
       </c>
       <c r="L9">
-        <v>2.9862279801774001E-4</v>
+        <v>0.0002986769367108244</v>
       </c>
       <c r="M9">
-        <v>2.1465450714923241E-4</v>
+        <v>0.0002146797923201637</v>
       </c>
       <c r="N9">
-        <v>2.1529370643740559E-4</v>
+        <v>0.0002153190156980401</v>
       </c>
       <c r="O9">
-        <v>3.65365951380727E-4</v>
+        <v>0.0003654569847387032</v>
       </c>
       <c r="P9">
-        <v>3.5613485469915219E-4</v>
+        <v>0.0003561989969207282</v>
       </c>
       <c r="Q9">
-        <v>2.9264796262629328E-4</v>
+        <v>0.0002926952298781901</v>
       </c>
       <c r="R9">
-        <v>3.8757038474724351E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.0003876414819374874</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1048,55 +988,55 @@
         <v>25</v>
       </c>
       <c r="C10">
-        <v>1.7667385205740431E-4</v>
+        <v>0.0001766532438781271</v>
       </c>
       <c r="D10">
-        <v>1.931028859369318E-5</v>
+        <v>1.930788550179934E-05</v>
       </c>
       <c r="E10">
-        <v>1.157177549654104E-2</v>
+        <v>0.01157129552496307</v>
       </c>
       <c r="F10">
-        <v>1.120433381169566E-4</v>
+        <v>0.0001120303379313476</v>
       </c>
       <c r="G10">
-        <v>1.482920712210456E-2</v>
+        <v>0.01482866575584448</v>
       </c>
       <c r="H10">
-        <v>1.5989823990204301E-2</v>
+        <v>0.01598926613196335</v>
       </c>
       <c r="I10">
-        <v>1.091678493772331E-3</v>
+        <v>0.001091565316617035</v>
       </c>
       <c r="J10">
-        <v>1.3229488375696661E-2</v>
+        <v>0.01322897550667238</v>
       </c>
       <c r="K10">
-        <v>8.3978479926169892E-5</v>
+        <v>8.396995826574704E-05</v>
       </c>
       <c r="L10">
-        <v>1.0302479613325469E-4</v>
+        <v>0.0001030121734561216</v>
       </c>
       <c r="M10">
-        <v>1.8776582998719569E-2</v>
+        <v>0.01877598413120405</v>
       </c>
       <c r="N10">
-        <v>1.894392821316437E-2</v>
+        <v>0.01894332933687399</v>
       </c>
       <c r="O10">
-        <v>1.114063222016228E-4</v>
+        <v>0.0001113903521253362</v>
       </c>
       <c r="P10">
-        <v>1.8213738674084261E-4</v>
+        <v>0.0001821134188787079</v>
       </c>
       <c r="Q10">
-        <v>5.4133727691295071E-3</v>
+        <v>0.005413053409602291</v>
       </c>
       <c r="R10">
-        <v>3.7793035009289869E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.0003778835080471535</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1104,55 +1044,55 @@
         <v>26</v>
       </c>
       <c r="C11">
-        <v>1.659140608165451E-4</v>
+        <v>0.0001658944660392599</v>
       </c>
       <c r="D11">
-        <v>9.1851637252430892E-3</v>
+        <v>0.009184428511043756</v>
       </c>
       <c r="E11">
-        <v>3.1251628903170821E-3</v>
+        <v>0.00312472649382599</v>
       </c>
       <c r="F11">
-        <v>7.2289441868299284E-3</v>
+        <v>0.007228297761548016</v>
       </c>
       <c r="G11">
-        <v>1.805212631302493E-3</v>
+        <v>0.001804906026336751</v>
       </c>
       <c r="H11">
-        <v>1.862984792065716E-3</v>
+        <v>0.001862671889387795</v>
       </c>
       <c r="I11">
-        <v>1.189876961310387E-2</v>
+        <v>0.01189788335785913</v>
       </c>
       <c r="J11">
-        <v>2.5042739274536261E-3</v>
+        <v>0.002503893903211111</v>
       </c>
       <c r="K11">
-        <v>2.4801244124213529E-3</v>
+        <v>0.00247980465075173</v>
       </c>
       <c r="L11">
-        <v>8.3699316782900029E-3</v>
+        <v>0.008369218361689818</v>
       </c>
       <c r="M11">
-        <v>1.1283677531876289E-3</v>
+        <v>0.001128146516952069</v>
       </c>
       <c r="N11">
-        <v>1.100965330701647E-3</v>
+        <v>0.001100748704522391</v>
       </c>
       <c r="O11">
-        <v>4.5671109887938741E-3</v>
+        <v>0.004566645381953153</v>
       </c>
       <c r="P11">
-        <v>1.306290498341723E-2</v>
+        <v>0.01306197034510394</v>
       </c>
       <c r="Q11">
-        <v>5.5246633413695316E-3</v>
+        <v>0.005524069413440999</v>
       </c>
       <c r="R11">
-        <v>9.1492212510447014E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.00914847338394076</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1160,55 +1100,55 @@
         <v>27</v>
       </c>
       <c r="C12">
-        <v>1.7835215813046359E-5</v>
+        <v>1.783382031004539E-05</v>
       </c>
       <c r="D12">
-        <v>6.2878173471385658E-6</v>
+        <v>6.287897953529778E-06</v>
       </c>
       <c r="E12">
-        <v>1.4503232126307879E-4</v>
+        <v>0.0001450351599651111</v>
       </c>
       <c r="F12">
-        <v>3.2016785255358208E-5</v>
+        <v>3.201704203336858E-05</v>
       </c>
       <c r="G12">
-        <v>1.096842896862469E-4</v>
+        <v>0.0001096863448746533</v>
       </c>
       <c r="H12">
-        <v>8.7356599529969068E-5</v>
+        <v>8.735849789578432E-05</v>
       </c>
       <c r="I12">
-        <v>1.4825914233997011E-4</v>
+        <v>0.000148261814127173</v>
       </c>
       <c r="J12">
-        <v>1.228007950179797E-4</v>
+        <v>0.0001228031786338798</v>
       </c>
       <c r="K12">
-        <v>1.104893044494625E-5</v>
+        <v>1.104888452355482E-05</v>
       </c>
       <c r="L12">
-        <v>9.9215842737360424E-5</v>
+        <v>9.92166041097119E-05</v>
       </c>
       <c r="M12">
-        <v>9.4868646103060051E-5</v>
+        <v>9.487067617424513E-05</v>
       </c>
       <c r="N12">
-        <v>1.018848393403335E-4</v>
+        <v>0.0001018870227140946</v>
       </c>
       <c r="O12">
-        <v>4.5490289602048107E-3</v>
+        <v>0.004549025181889012</v>
       </c>
       <c r="P12">
-        <v>8.4897569358225507E-5</v>
+        <v>8.489884940267955E-05</v>
       </c>
       <c r="Q12">
-        <v>1.367767527252431E-4</v>
+        <v>0.0001367788077105176</v>
       </c>
       <c r="R12">
-        <v>3.9341480581531798E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.0003934176001137476</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1216,55 +1156,55 @@
         <v>28</v>
       </c>
       <c r="C13">
-        <v>1.7057458280791048E-5</v>
+        <v>1.705631768286339E-05</v>
       </c>
       <c r="D13">
-        <v>2.0687203265528389E-5</v>
+        <v>2.068673985726743E-05</v>
       </c>
       <c r="E13">
-        <v>2.062603850470335E-4</v>
+        <v>0.0002062531918566312</v>
       </c>
       <c r="F13">
-        <v>7.9758457211053188E-5</v>
+        <v>7.975645913508229E-05</v>
       </c>
       <c r="G13">
-        <v>3.0127214450429622E-4</v>
+        <v>0.0003012617771695023</v>
       </c>
       <c r="H13">
-        <v>1.5995020701855709E-4</v>
+        <v>0.0001599451513905951</v>
       </c>
       <c r="I13">
-        <v>3.962801899185911E-4</v>
+        <v>0.0003962669244936848</v>
       </c>
       <c r="J13">
-        <v>2.048450166656274E-4</v>
+        <v>0.0002048375019236836</v>
       </c>
       <c r="K13">
-        <v>3.3198996785196907E-5</v>
+        <v>3.319845567416679E-05</v>
       </c>
       <c r="L13">
-        <v>4.9150171414867833E-4</v>
+        <v>0.0004914875813265394</v>
       </c>
       <c r="M13">
-        <v>1.3398189013783419E-4</v>
+        <v>0.000133977522736995</v>
       </c>
       <c r="N13">
-        <v>9.4408790915390562E-5</v>
+        <v>9.44056807257101E-05</v>
       </c>
       <c r="O13">
-        <v>3.1259579412909293E-4</v>
+        <v>0.0003125786063758912</v>
       </c>
       <c r="P13">
-        <v>1.5341438411637131E-3</v>
+        <v>0.001534102562128504</v>
       </c>
       <c r="Q13">
-        <v>1.012694750976424E-3</v>
+        <v>0.001012667613742529</v>
       </c>
       <c r="R13">
-        <v>3.8809647877379198E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.0003880804928257794</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1272,55 +1212,55 @@
         <v>29</v>
       </c>
       <c r="C14">
-        <v>1.1370028824155081E-3</v>
+        <v>0.001136904314206343</v>
       </c>
       <c r="D14">
-        <v>7.1570554805572853E-2</v>
+        <v>0.0715720338673748</v>
       </c>
       <c r="E14">
-        <v>6.9850956387406946E-2</v>
+        <v>0.06985234229298032</v>
       </c>
       <c r="F14">
-        <v>7.1222265736191795E-2</v>
+        <v>0.071223756577245</v>
       </c>
       <c r="G14">
-        <v>6.8246865845788665E-2</v>
+        <v>0.06824821434485165</v>
       </c>
       <c r="H14">
-        <v>6.7670940153512035E-2</v>
+        <v>0.06767228481642512</v>
       </c>
       <c r="I14">
-        <v>7.5921730610225419E-2</v>
+        <v>0.07592315641341041</v>
       </c>
       <c r="J14">
-        <v>6.9883888586175821E-2</v>
+        <v>0.06988526625023059</v>
       </c>
       <c r="K14">
-        <v>6.8526482317091436E-2</v>
+        <v>0.0685279796058457</v>
       </c>
       <c r="L14">
-        <v>7.2735564951105294E-2</v>
+        <v>0.07273702766538635</v>
       </c>
       <c r="M14">
-        <v>6.6439636518654338E-2</v>
+        <v>0.06644096084610367</v>
       </c>
       <c r="N14">
-        <v>6.6652205578018875E-2</v>
+        <v>0.06665353377237294</v>
       </c>
       <c r="O14">
-        <v>8.1400521054314889E-2</v>
+        <v>0.08140210301851634</v>
       </c>
       <c r="P14">
-        <v>7.3466200179760147E-2</v>
+        <v>0.07346756150259343</v>
       </c>
       <c r="Q14">
-        <v>7.1936284365880843E-2</v>
+        <v>0.07193764957008073</v>
       </c>
       <c r="R14">
-        <v>7.8139065774272459E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.07814054947622191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1328,55 +1268,55 @@
         <v>30</v>
       </c>
       <c r="C15">
-        <v>3.0248557660161548E-4</v>
+        <v>0.0003025021335428447</v>
       </c>
       <c r="D15">
-        <v>1.589790388835814E-3</v>
+        <v>0.001589391344802924</v>
       </c>
       <c r="E15">
-        <v>1.435971370044426E-3</v>
+        <v>0.001435506972191089</v>
       </c>
       <c r="F15">
-        <v>1.711780311470629E-3</v>
+        <v>0.001711381234627614</v>
       </c>
       <c r="G15">
-        <v>1.5394621432903151E-3</v>
+        <v>0.001539003155046372</v>
       </c>
       <c r="H15">
-        <v>1.5047820434925801E-3</v>
+        <v>0.001504338144257612</v>
       </c>
       <c r="I15">
-        <v>9.5537243034449259E-4</v>
+        <v>0.0009548566945482333</v>
       </c>
       <c r="J15">
-        <v>1.4199794214740269E-3</v>
+        <v>0.001419509083592423</v>
       </c>
       <c r="K15">
-        <v>2.275800347997244E-3</v>
+        <v>0.002275470606269415</v>
       </c>
       <c r="L15">
-        <v>1.4893155209244799E-3</v>
+        <v>0.001488864979653246</v>
       </c>
       <c r="M15">
-        <v>1.569305144242978E-3</v>
+        <v>0.001568865663182009</v>
       </c>
       <c r="N15">
-        <v>1.5474079698005051E-3</v>
+        <v>0.001546968500241594</v>
       </c>
       <c r="O15">
-        <v>1.177802539497142E-3</v>
+        <v>0.001177182406746363</v>
       </c>
       <c r="P15">
-        <v>1.105995553499632E-3</v>
+        <v>0.001105480166113479</v>
       </c>
       <c r="Q15">
-        <v>1.3361818402092881E-3</v>
+        <v>0.001335701175835653</v>
       </c>
       <c r="R15">
-        <v>9.6200098753097948E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.0009614635557211661</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1384,55 +1324,55 @@
         <v>31</v>
       </c>
       <c r="C16">
-        <v>9.576508847505611E-6</v>
+        <v>9.575287935485787E-06</v>
       </c>
       <c r="D16">
-        <v>6.0300100492673824E-3</v>
+        <v>0.006029715858859684</v>
       </c>
       <c r="E16">
-        <v>6.2483275392546658E-3</v>
+        <v>0.006248023034381721</v>
       </c>
       <c r="F16">
-        <v>6.0182760880496218E-3</v>
+        <v>0.006017987207612831</v>
       </c>
       <c r="G16">
-        <v>6.2246821512988897E-3</v>
+        <v>0.006224376290607672</v>
       </c>
       <c r="H16">
-        <v>6.2448585956367576E-3</v>
+        <v>0.00624454496577515</v>
       </c>
       <c r="I16">
-        <v>5.9380543628394997E-3</v>
+        <v>0.00593777144490269</v>
       </c>
       <c r="J16">
-        <v>6.2439963717809679E-3</v>
+        <v>0.006243691677647802</v>
       </c>
       <c r="K16">
-        <v>5.8937722351182194E-3</v>
+        <v>0.005893482069810045</v>
       </c>
       <c r="L16">
-        <v>5.9481458426175002E-3</v>
+        <v>0.005947866949210766</v>
       </c>
       <c r="M16">
-        <v>6.2287356766396922E-3</v>
+        <v>0.006228420672956736</v>
       </c>
       <c r="N16">
-        <v>6.2291265872481544E-3</v>
+        <v>0.006228810662881473</v>
       </c>
       <c r="O16">
-        <v>5.0918518118878648E-3</v>
+        <v>0.005091630516607946</v>
       </c>
       <c r="P16">
-        <v>5.8816123768142201E-3</v>
+        <v>0.005881337705870081</v>
       </c>
       <c r="Q16">
-        <v>6.061232463659744E-3</v>
+        <v>0.006060939410885274</v>
       </c>
       <c r="R16">
-        <v>5.7311435420790572E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.005730878450787838</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1440,55 +1380,55 @@
         <v>32</v>
       </c>
       <c r="C17">
-        <v>4.8130367341329157E-5</v>
+        <v>4.811262956309266E-05</v>
       </c>
       <c r="D17">
-        <v>3.7503473849275153E-2</v>
+        <v>0.03750709058007516</v>
       </c>
       <c r="E17">
-        <v>3.9157885860188119E-2</v>
+        <v>0.0391616220566412</v>
       </c>
       <c r="F17">
-        <v>3.862145510414583E-2</v>
+        <v>0.03862521171970517</v>
       </c>
       <c r="G17">
-        <v>4.068416192250221E-2</v>
+        <v>0.04068798308769523</v>
       </c>
       <c r="H17">
-        <v>4.10681587313729E-2</v>
+        <v>0.0410719145391513</v>
       </c>
       <c r="I17">
-        <v>3.1409221298638899E-2</v>
+        <v>0.03141249012751156</v>
       </c>
       <c r="J17">
-        <v>3.9187968587976317E-2</v>
+        <v>0.03919170783846512</v>
       </c>
       <c r="K17">
-        <v>4.3555322317723938E-2</v>
+        <v>0.04355932261816542</v>
       </c>
       <c r="L17">
-        <v>3.6266244747973138E-2</v>
+        <v>0.03626993790123752</v>
       </c>
       <c r="M17">
-        <v>4.2116410145519298E-2</v>
+        <v>0.04212020664553012</v>
       </c>
       <c r="N17">
-        <v>4.1954973456976838E-2</v>
+        <v>0.04195874617713891</v>
       </c>
       <c r="O17">
-        <v>2.818879177609818E-2</v>
+        <v>0.02819203596573915</v>
       </c>
       <c r="P17">
-        <v>3.2663142560533202E-2</v>
+        <v>0.0326666191160646</v>
       </c>
       <c r="Q17">
-        <v>3.6676973884936792E-2</v>
+        <v>0.03668061325563959</v>
       </c>
       <c r="R17">
-        <v>3.044770482911351E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+        <v>0.03045100067425055</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1496,52 +1436,52 @@
         <v>33</v>
       </c>
       <c r="C18">
-        <v>2.9021109402804372E-4</v>
+        <v>0.0002901867544696206</v>
       </c>
       <c r="D18">
-        <v>1.541598092263622E-3</v>
+        <v>0.001541870439652471</v>
       </c>
       <c r="E18">
-        <v>1.891371519613212E-3</v>
+        <v>0.001891615177542756</v>
       </c>
       <c r="F18">
-        <v>2.1244357548661158E-3</v>
+        <v>0.002124735516122556</v>
       </c>
       <c r="G18">
-        <v>2.5552797980205951E-3</v>
+        <v>0.00255553943149477</v>
       </c>
       <c r="H18">
-        <v>2.6759779398678111E-3</v>
+        <v>0.002676233143587772</v>
       </c>
       <c r="I18">
-        <v>1.267043780641262E-3</v>
+        <v>0.001266887959895731</v>
       </c>
       <c r="J18">
-        <v>1.947941044669232E-3</v>
+        <v>0.001948184315639379</v>
       </c>
       <c r="K18">
-        <v>4.8722856970676012E-3</v>
+        <v>0.004872686071876017</v>
       </c>
       <c r="L18">
-        <v>9.5936291769314387E-4</v>
+        <v>0.0009596225146133777</v>
       </c>
       <c r="M18">
-        <v>3.129300911663138E-3</v>
+        <v>0.003129564430272361</v>
       </c>
       <c r="N18">
-        <v>3.0804417723250608E-3</v>
+        <v>0.003080702919521695</v>
       </c>
       <c r="O18">
-        <v>9.3124207424912658E-4</v>
+        <v>0.0009310521522316164</v>
       </c>
       <c r="P18">
-        <v>1.084506704571789E-3</v>
+        <v>0.001084333332943217</v>
       </c>
       <c r="Q18">
-        <v>8.591105207830025E-4</v>
+        <v>0.0008593356433594947</v>
       </c>
       <c r="R18">
-        <v>1.1899764627124781E-3</v>
+        <v>0.001189802800421076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>